<commit_message>
Continuo proyecto gestor de actuaciones
</commit_message>
<xml_diff>
--- a/proyectos/gestorDeActuaciones/src/pruebasExcel/olin.xlsx
+++ b/proyectos/gestorDeActuaciones/src/pruebasExcel/olin.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t xml:space="preserve">Código Cliente</t>
   </si>
@@ -183,6 +183,18 @@
   </si>
   <si>
     <t xml:space="preserve">Juanito Fdez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">preguntas:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.- Todo estos campos se exportan o algunos los gestiono yo. Ej: tipo, nivel, accion, estado, fecha citacion, incidencia atendida, fecha atendida,  hora atendida, fecha cerrada, hora cerrada, usuario cerrada, motivo de erro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.- Las cabeceras son nombres definitivos, necesito que lo sean respentando todos los caracteres, espacios, tildes, …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.- Entiendo que el codigo incidencia será unico. Lo necesitaría para no introducir en la base de datos incidencias repetidas</t>
   </si>
 </sst>
 </file>
@@ -360,10 +372,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AB11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y3" activeCellId="0" sqref="Y3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -516,6 +528,26 @@
         <v>266000</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>